<commit_message>
ajustes de reportes backend
</commit_message>
<xml_diff>
--- a/docs/formatos/ListadoParticipantes.xlsx
+++ b/docs/formatos/ListadoParticipantes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Usuario</t>
   </si>
@@ -66,17 +66,20 @@
     <t xml:space="preserve">Empresa: YYYYYYYYYY. </t>
   </si>
   <si>
-    <t>Activo</t>
-  </si>
-  <si>
     <t>Logueado</t>
+  </si>
+  <si>
+    <t>Hora registro</t>
+  </si>
+  <si>
+    <t>Acceso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +114,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -143,12 +153,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -173,6 +222,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -459,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,45 +532,45 @@
     <col min="2" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -522,7 +583,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -535,45 +596,48 @@
       <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -581,6 +645,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
agregando campo clave a listados de participantes
</commit_message>
<xml_diff>
--- a/docs/formatos/ListadoParticipantes.xlsx
+++ b/docs/formatos/ListadoParticipantes.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\formacion2.0\docs\formatos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Usuario</t>
   </si>
@@ -73,12 +78,15 @@
   </si>
   <si>
     <t>Acceso</t>
+  </si>
+  <si>
+    <t>Clave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,26 +528,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1"/>
-    <col min="7" max="7" width="40.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
@@ -554,8 +562,9 @@
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
-    <row r="2" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
@@ -570,8 +579,9 @@
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -583,63 +593,67 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -647,11 +661,12 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>